<commit_message>
Changed label of 'address'
</commit_message>
<xml_diff>
--- a/Household.xlsx
+++ b/Household.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilytunggala/Desktop/1H2018/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilytunggala/Desktop/XLSForm Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -231,9 +231,6 @@
     <t>address</t>
   </si>
   <si>
-    <t>Location of the house</t>
-  </si>
-  <si>
     <t>geopoint</t>
   </si>
   <si>
@@ -430,6 +427,9 @@
   </si>
   <si>
     <t>land</t>
+  </si>
+  <si>
+    <t>Location of house</t>
   </si>
 </sst>
 </file>
@@ -796,9 +796,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -816,7 +816,7 @@
         <v>50</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>24</v>
@@ -838,13 +838,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>56</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>57</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -852,29 +852,29 @@
         <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
         <v>61</v>
       </c>
-      <c r="B5" t="s">
-        <v>62</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" t="s">
         <v>64</v>
-      </c>
-      <c r="B6" t="s">
-        <v>65</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>37</v>
@@ -882,57 +882,57 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="s">
         <v>66</v>
       </c>
-      <c r="B7" t="s">
-        <v>67</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" t="s">
         <v>75</v>
       </c>
-      <c r="B11" t="s">
-        <v>76</v>
-      </c>
       <c r="C11" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -940,32 +940,32 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" t="s">
         <v>83</v>
       </c>
-      <c r="B14" t="s">
-        <v>84</v>
-      </c>
       <c r="C14" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -973,21 +973,21 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -995,15 +995,15 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
         <v>32</v>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
@@ -1085,7 +1085,7 @@
         <v>50</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1104,7 +1104,7 @@
         <v>52</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>1</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -1123,10 +1123,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
         <v>39</v>
@@ -1134,10 +1134,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C6" t="s">
         <v>40</v>
@@ -1145,10 +1145,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C7" t="s">
         <v>41</v>
@@ -1156,10 +1156,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
         <v>42</v>
@@ -1167,10 +1167,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C9" t="s">
         <v>43</v>
@@ -1178,10 +1178,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" t="s">
         <v>44</v>
@@ -1189,10 +1189,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C11" t="s">
         <v>45</v>
@@ -1200,10 +1200,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C12" t="s">
         <v>46</v>
@@ -1211,10 +1211,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -1222,10 +1222,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -1233,10 +1233,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -1244,10 +1244,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
@@ -1255,10 +1255,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -1266,10 +1266,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
@@ -1277,10 +1277,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
@@ -1288,10 +1288,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
@@ -1302,7 +1302,7 @@
         <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C21" t="s">
         <v>12</v>
@@ -1313,7 +1313,7 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C22" t="s">
         <v>13</v>
@@ -1324,7 +1324,7 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C23" t="s">
         <v>14</v>
@@ -1335,7 +1335,7 @@
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C24" t="s">
         <v>15</v>
@@ -1346,7 +1346,7 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C25" t="s">
         <v>16</v>
@@ -1357,7 +1357,7 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C26" t="s">
         <v>17</v>
@@ -1368,7 +1368,7 @@
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
@@ -1379,7 +1379,7 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C28" t="s">
         <v>19</v>
@@ -1395,7 +1395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
@@ -1414,7 +1414,7 @@
         <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>3</v>
@@ -1422,16 +1422,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" t="s">
         <v>89</v>
-      </c>
-      <c r="B2" t="s">
-        <v>90</v>
       </c>
       <c r="C2">
         <v>2018061401</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>